<commit_message>
Mise a jour du schéma
Rajout et création des éléments manquant sur Altium, documentation et remplissage du carnet journalier
</commit_message>
<xml_diff>
--- a/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
+++ b/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/alexandre_bourquenoud_studentfr_ch/Documents/PHIE/jeu_du_moulin_alexandre_bourquenoud/jeu_du_moulin_2025_boura/jeu_du_moulin_boura/rpt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="320" documentId="13_ncr:1_{C89F1C62-A35A-4363-963D-04F3CDCC9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D74B0967-F63B-44A6-9CE8-EF702C402728}"/>
+  <xr:revisionPtr revIDLastSave="423" documentId="13_ncr:1_{C89F1C62-A35A-4363-963D-04F3CDCC9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95BE638E-CE68-4383-B7B6-EA4E6ADC2A92}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -129,6 +129,39 @@
   </si>
   <si>
     <t>mise en place de l'environnement de travail du projet</t>
+  </si>
+  <si>
+    <t>quelques problème avec l'implémentation de l'utilisation de Github à cause d'une erreur de setup que j'ai fait avec les repositories -&gt; j'ai résolue le problème en créant correctement les repositories</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Sauvegarde des fichiers qui m'on été fourni en avance sur le projet Github</t>
+  </si>
+  <si>
+    <t>FWR</t>
+  </si>
+  <si>
+    <t>Discussion avec Monsieur Eglis au sujet du proogramme Cube pour la programmation sur STM32 et installation de celui-ci</t>
+  </si>
+  <si>
+    <t>SCH</t>
+  </si>
+  <si>
+    <t>rédaction de la documentation avec des informations lié au projet.</t>
+  </si>
+  <si>
+    <t>Rédaction du journal de travail</t>
+  </si>
+  <si>
+    <t>J'ai pris un bon moment pour faire le symbole de l'uC</t>
+  </si>
+  <si>
+    <t>Avancement du schéma -&gt; changement d'IC, ajout  des LEDs manquantes, création des symboles manquants, schématisation des condensateurs de découplage et des matrices de LEDs et de touches capacitives</t>
   </si>
 </sst>
 </file>
@@ -314,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -406,18 +439,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -442,319 +463,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1388,18 +1119,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N7" sqref="N6:N7"/>
+      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="35" style="1" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
@@ -1434,19 +1165,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1457,11 +1188,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -1469,8 +1200,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1482,84 +1213,132 @@
       <c r="D5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="13"/>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="13"/>
+      <c r="F6" s="13">
+        <v>0.5</v>
+      </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="44"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="13"/>
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="40"/>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.9</v>
+      </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="6"/>
+    <row r="8" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="40"/>
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="13">
+        <v>0.7</v>
+      </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+    <row r="9" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="40"/>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6">
+        <v>0.4</v>
+      </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="6"/>
+    <row r="10" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="40"/>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="6">
+        <v>3.5</v>
+      </c>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31">
+    <row r="11" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="40"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="31">
         <v>45789</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="18">
-        <f>SUM(F5:F10)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="F12" s="18">
+        <f>SUM(F5:F11)</f>
+        <v>7</v>
+      </c>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1568,7 +1347,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1577,7 +1356,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1585,35 +1364,35 @@
       <c r="F15" s="6"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31">
+    <row r="16" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="40"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="31">
         <v>45790</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="18">
-        <f>SUM(F12:F15)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="F17" s="18">
+        <f>SUM(F13:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1622,7 +1401,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1631,7 +1410,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1639,35 +1418,35 @@
       <c r="F20" s="6"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31">
+    <row r="21" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="40"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="31">
         <v>45791</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="18">
-        <f>SUM(F17:F20)</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="F22" s="18">
+        <f>SUM(F18:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1676,7 +1455,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1685,7 +1464,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1693,35 +1472,35 @@
       <c r="F25" s="6"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="31">
+    <row r="26" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="40"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="31">
         <v>45792</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="18">
-        <f>SUM(F22:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
+      <c r="F27" s="18">
+        <f>SUM(F23:F26)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1730,7 +1509,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1739,7 +1518,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1747,78 +1526,78 @@
       <c r="F30" s="6"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31">
+    <row r="31" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="40"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="31">
         <v>45793</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="20" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="21">
-        <f>SUM(F27:F30)</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
+      <c r="F32" s="21">
+        <f>SUM(F28:F31)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17" t="s">
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="22">
-        <f>F11+F16+F21+F26+F31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37" t="s">
+      <c r="G33" s="22">
+        <f>F12+F17+F22+F27+F32</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="35"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="10"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
@@ -1827,7 +1606,7 @@
       <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
@@ -1836,7 +1615,7 @@
       <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
@@ -1845,7 +1624,7 @@
       <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
@@ -1854,7 +1633,7 @@
       <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="25"/>
       <c r="C43" s="25"/>
       <c r="D43" s="25"/>
@@ -1863,25 +1642,25 @@
       <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="28"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="26"/>
       <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="26"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="28"/>
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
       <c r="D46" s="25"/>
@@ -1890,7 +1669,7 @@
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
+      <c r="A47" s="44"/>
       <c r="B47" s="25"/>
       <c r="C47" s="25"/>
       <c r="D47" s="25"/>
@@ -1899,7 +1678,7 @@
       <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
       <c r="D48" s="25"/>
@@ -1908,25 +1687,25 @@
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="28"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="26"/>
       <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="26"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="28"/>
       <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
+      <c r="A51" s="44"/>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
       <c r="D51" s="25"/>
@@ -1935,7 +1714,7 @@
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
+      <c r="A52" s="44"/>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
       <c r="D52" s="25"/>
@@ -1944,7 +1723,7 @@
       <c r="G52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="35"/>
+      <c r="A53" s="44"/>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
       <c r="D53" s="25"/>
@@ -1953,25 +1732,25 @@
       <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="28"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="26"/>
       <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="35"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="26"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="28"/>
       <c r="G55" s="10"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
+      <c r="A56" s="44"/>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
@@ -1980,7 +1759,7 @@
       <c r="G56" s="10"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="35"/>
+      <c r="A57" s="44"/>
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
       <c r="D57" s="25"/>
@@ -1989,7 +1768,7 @@
       <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
+      <c r="A58" s="44"/>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
       <c r="D58" s="25"/>
@@ -1998,25 +1777,25 @@
       <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="24"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="28"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="26"/>
       <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="26"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="28"/>
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="A61" s="44"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
@@ -2025,7 +1804,7 @@
       <c r="G61" s="10"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
+      <c r="A62" s="44"/>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
       <c r="D62" s="25"/>
@@ -2034,7 +1813,7 @@
       <c r="G62" s="10"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
+      <c r="A63" s="44"/>
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
       <c r="D63" s="25"/>
@@ -2043,89 +1822,98 @@
       <c r="G63" s="10"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="24"/>
-      <c r="B64" s="29"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="28"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="26"/>
       <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="28"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="34"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="34"/>
+      <c r="A66" s="41"/>
+      <c r="B66" s="41"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="28"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="43"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="A34:G34"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A33:D33"/>
   </mergeCells>
-  <conditionalFormatting sqref="F38:F64">
-    <cfRule type="containsText" dxfId="57" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",F38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",F38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G65">
-    <cfRule type="containsText" dxfId="53" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G65)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G65)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F31">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="F5:F32">
+    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G32)))</formula>
+  <conditionalFormatting sqref="F39:F65">
+    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",F39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G32)))</formula>
+    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",F39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",G33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",G33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",G66)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",G66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2181,19 +1969,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2204,11 +1992,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2217,7 +2005,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2228,7 +2016,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2237,7 +2025,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2246,7 +2034,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2255,7 +2043,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2264,7 +2052,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2289,7 +2077,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2300,7 +2088,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2309,7 +2097,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2318,7 +2106,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2343,7 +2131,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2355,7 +2143,7 @@
       <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2364,7 +2152,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2373,7 +2161,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2398,7 +2186,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2409,7 +2197,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2419,7 +2207,7 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2429,7 +2217,7 @@
       <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2454,7 +2242,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -2465,7 +2253,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2474,7 +2262,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2483,7 +2271,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2508,12 +2296,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:10" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -2524,15 +2312,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2612,19 +2400,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2635,11 +2423,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2648,7 +2436,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2659,7 +2447,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2668,7 +2456,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2677,7 +2465,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2686,7 +2474,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2695,7 +2483,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2720,7 +2508,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2731,7 +2519,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2740,7 +2528,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2749,7 +2537,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2774,7 +2562,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2785,7 +2573,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2794,7 +2582,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2803,7 +2591,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2828,7 +2616,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2839,7 +2627,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2848,7 +2636,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2857,7 +2645,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2882,7 +2670,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -2893,7 +2681,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2902,7 +2690,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2911,7 +2699,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2936,12 +2724,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -2952,18 +2740,23 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -2971,11 +2764,6 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Terminé">
@@ -3038,19 +2826,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3061,11 +2849,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3074,7 +2862,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3085,7 +2873,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3094,7 +2882,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3103,7 +2891,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3112,7 +2900,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3121,7 +2909,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3146,7 +2934,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3157,7 +2945,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3166,7 +2954,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3175,7 +2963,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3200,7 +2988,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3211,7 +2999,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3220,7 +3008,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3229,7 +3017,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3254,7 +3042,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3265,7 +3053,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3274,7 +3062,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3283,7 +3071,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3308,7 +3096,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3319,7 +3107,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3328,7 +3116,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3337,7 +3125,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3362,12 +3150,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3378,18 +3166,23 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -3397,11 +3190,6 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Terminé">
@@ -3464,19 +3252,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3487,11 +3275,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3500,7 +3288,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3511,7 +3299,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3520,7 +3308,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3529,7 +3317,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3538,7 +3326,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3547,7 +3335,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3572,7 +3360,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3583,7 +3371,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3592,7 +3380,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3601,7 +3389,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3626,7 +3414,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3637,7 +3425,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3646,7 +3434,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3655,7 +3443,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3680,7 +3468,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3691,7 +3479,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3700,7 +3488,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3709,7 +3497,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3734,7 +3522,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3745,7 +3533,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3754,7 +3542,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3763,7 +3551,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3788,12 +3576,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3804,15 +3592,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3892,19 +3680,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3915,11 +3703,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3928,7 +3716,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3939,7 +3727,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3948,7 +3736,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3957,7 +3745,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3966,7 +3754,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3975,7 +3763,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4000,7 +3788,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -4011,7 +3799,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -4020,7 +3808,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -4029,7 +3817,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -4054,7 +3842,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -4065,7 +3853,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -4074,7 +3862,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -4083,7 +3871,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -4108,7 +3896,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -4119,7 +3907,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -4128,7 +3916,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4137,7 +3925,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4162,7 +3950,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -4173,7 +3961,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4182,7 +3970,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4191,7 +3979,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4216,12 +4004,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4232,15 +4020,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4318,19 +4106,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -4341,11 +4129,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -4354,7 +4142,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -4365,7 +4153,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4374,7 +4162,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4383,7 +4171,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -4392,7 +4180,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4401,7 +4189,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4426,7 +4214,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -4437,7 +4225,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -4446,7 +4234,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -4455,7 +4243,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -4480,7 +4268,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -4491,7 +4279,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -4500,7 +4288,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -4509,7 +4297,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -4534,7 +4322,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -4545,7 +4333,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -4554,7 +4342,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4563,7 +4351,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4588,7 +4376,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -4599,7 +4387,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4608,7 +4396,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4617,7 +4405,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4642,12 +4430,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4658,15 +4446,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
changement du schéma Altium
changement de plusieurs éléments sur altium ce qui nous rapproche de la version "fonctionnel" (en théorie)
</commit_message>
<xml_diff>
--- a/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
+++ b/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/alexandre_bourquenoud_studentfr_ch/Documents/PHIE/jeu_du_moulin_alexandre_bourquenoud/jeu_du_moulin_2025_boura/jeu_du_moulin_boura/rpt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="423" documentId="13_ncr:1_{C89F1C62-A35A-4363-963D-04F3CDCC9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95BE638E-CE68-4383-B7B6-EA4E6ADC2A92}"/>
+  <xr:revisionPtr revIDLastSave="476" documentId="13_ncr:1_{C89F1C62-A35A-4363-963D-04F3CDCC9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84A218C9-2E24-4A84-924B-E0D295C4F96D}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,21 @@
   </si>
   <si>
     <t>Avancement du schéma -&gt; changement d'IC, ajout  des LEDs manquantes, création des symboles manquants, schématisation des condensateurs de découplage et des matrices de LEDs et de touches capacitives</t>
+  </si>
+  <si>
+    <t>Avancement du schéma -&gt; changement de l'utilisation des pins du uC avec l'utilisation de STM32CubeIDE pour savoir lesquelles sont utiles</t>
+  </si>
+  <si>
+    <t>Conversation avec M.Eglis sur l'utilisation du logiciel de programmation STM32CubeIDE pour me montrer son fonctionnement</t>
+  </si>
+  <si>
+    <t>Correction de la BOM avec les composants nécessaires</t>
+  </si>
+  <si>
+    <t>dimensionnement des composants pour le régulateur de tension 3.3V</t>
+  </si>
+  <si>
+    <t>création de certaines empreintes manquantes</t>
   </si>
 </sst>
 </file>
@@ -439,6 +454,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -461,18 +488,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -856,6 +871,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -1119,11 +1138,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <pane ySplit="4" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1165,19 +1184,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1188,11 +1207,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -1201,7 +1220,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1222,7 +1241,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1239,7 +1258,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -1258,7 +1277,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1275,7 +1294,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1292,7 +1311,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1311,7 +1330,7 @@
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1335,82 +1354,128 @@
       </c>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
+    <row r="13" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6">
+        <v>4</v>
+      </c>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+    <row r="14" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="44"/>
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6">
+        <v>0.5</v>
+      </c>
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6">
+        <v>1.5</v>
+      </c>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+    <row r="16" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="44"/>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6">
+        <v>0.5</v>
+      </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="31">
+    <row r="17" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="44"/>
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="31">
         <v>45790</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="18">
-        <f>SUM(F13:F16)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
+      <c r="F19" s="18">
+        <f>SUM(F13:F18)</f>
         <v>7</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="6"/>
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
+      <c r="A20" s="43" t="s">
+        <v>7</v>
+      </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1419,7 +1484,7 @@
       <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1427,26 +1492,17 @@
       <c r="F21" s="6"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31">
-        <v>45791</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="18">
-        <f>SUM(F18:F21)</f>
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="44"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="39" t="s">
-        <v>8</v>
-      </c>
+      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1454,17 +1510,26 @@
       <c r="F23" s="6"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="40"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="6"/>
+    <row r="24" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="31">
+        <v>45791</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="18">
+        <f>SUM(F20:F23)</f>
+        <v>0</v>
+      </c>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
+      <c r="A25" s="43" t="s">
+        <v>8</v>
+      </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1473,7 +1538,7 @@
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="40"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1481,26 +1546,17 @@
       <c r="F26" s="6"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31">
-        <v>45792</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="18">
-        <f>SUM(F23:F26)</f>
-        <v>0</v>
-      </c>
+    <row r="27" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="44"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="39" t="s">
-        <v>9</v>
-      </c>
+      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1508,17 +1564,26 @@
       <c r="F28" s="6"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="6"/>
+    <row r="29" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="31">
+        <v>45792</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="18">
+        <f>SUM(F25:F28)</f>
+        <v>0</v>
+      </c>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
+      <c r="A30" s="43" t="s">
+        <v>9</v>
+      </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1527,7 +1592,7 @@
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1535,87 +1600,87 @@
       <c r="F31" s="6"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31">
+    <row r="32" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="44"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="44"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="31">
         <v>45793</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="20" t="s">
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="21">
-        <f>SUM(F28:F31)</f>
+      <c r="F34" s="21">
+        <f>SUM(F30:F33)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="38" t="s">
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17" t="s">
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="22">
-        <f>F12+F17+F22+F27+F32</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="33" t="s">
+      <c r="G35" s="22">
+        <f>F12+F19+F24+F29+F34</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="39"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="10"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="10"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
+      <c r="A41" s="33"/>
       <c r="B41" s="25"/>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
@@ -1624,7 +1689,7 @@
       <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
+      <c r="A42" s="33"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
@@ -1633,7 +1698,7 @@
       <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="25"/>
       <c r="C43" s="25"/>
       <c r="D43" s="25"/>
@@ -1642,7 +1707,7 @@
       <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="25"/>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
@@ -1651,16 +1716,16 @@
       <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="28"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="26"/>
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
       <c r="D46" s="25"/>
@@ -1669,16 +1734,16 @@
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="26"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="28"/>
       <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
       <c r="D48" s="25"/>
@@ -1687,7 +1752,7 @@
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
@@ -1696,16 +1761,16 @@
       <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="28"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="26"/>
       <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
       <c r="D51" s="25"/>
@@ -1714,16 +1779,16 @@
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="26"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
       <c r="D53" s="25"/>
@@ -1732,7 +1797,7 @@
       <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="25"/>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
@@ -1741,16 +1806,16 @@
       <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="28"/>
+      <c r="A55" s="33"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="26"/>
       <c r="G55" s="10"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
+      <c r="A56" s="33"/>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
@@ -1759,16 +1824,16 @@
       <c r="G56" s="10"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="26"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="28"/>
       <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
+      <c r="A58" s="33"/>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
       <c r="D58" s="25"/>
@@ -1777,7 +1842,7 @@
       <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
+      <c r="A59" s="33"/>
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
       <c r="D59" s="25"/>
@@ -1786,16 +1851,16 @@
       <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="28"/>
+      <c r="A60" s="33"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="26"/>
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
+      <c r="A61" s="33"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
@@ -1804,16 +1869,16 @@
       <c r="G61" s="10"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="26"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="28"/>
       <c r="G62" s="10"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
+      <c r="A63" s="33"/>
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
       <c r="D63" s="25"/>
@@ -1822,7 +1887,7 @@
       <c r="G63" s="10"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
+      <c r="A64" s="33"/>
       <c r="B64" s="25"/>
       <c r="C64" s="25"/>
       <c r="D64" s="25"/>
@@ -1831,60 +1896,78 @@
       <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="24"/>
-      <c r="B65" s="29"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="28"/>
+      <c r="A65" s="33"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="26"/>
       <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
-      <c r="B66" s="41"/>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="28"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="43"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="28"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="35"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A36:G36"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A63:A66"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F32">
+  <conditionalFormatting sqref="F19:F34 F5:F16">
     <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F5)))</formula>
     </cfRule>
@@ -1892,28 +1975,28 @@
       <formula>NOT(ISERROR(SEARCH("En cours",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F65">
+  <conditionalFormatting sqref="F41:F67">
     <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",F39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",F41)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",F39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",F41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
+  <conditionalFormatting sqref="G35">
     <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G35)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G66">
+  <conditionalFormatting sqref="G68">
     <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G68)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1969,19 +2052,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1992,11 +2075,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2005,7 +2088,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2016,7 +2099,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2025,7 +2108,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2034,7 +2117,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2043,7 +2126,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2052,7 +2135,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2077,7 +2160,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2088,7 +2171,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2097,7 +2180,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2106,7 +2189,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2131,7 +2214,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2143,7 +2226,7 @@
       <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2152,7 +2235,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2161,7 +2244,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2186,7 +2269,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2197,7 +2280,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2207,7 +2290,7 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="40"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2217,7 +2300,7 @@
       <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2242,7 +2325,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -2253,7 +2336,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2262,7 +2345,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2271,7 +2354,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2296,12 +2379,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:10" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -2312,15 +2395,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2400,19 +2483,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2423,11 +2506,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2436,7 +2519,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2447,7 +2530,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2456,7 +2539,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2465,7 +2548,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2474,7 +2557,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2483,7 +2566,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2508,7 +2591,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2519,7 +2602,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2528,7 +2611,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2537,7 +2620,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2562,7 +2645,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2573,7 +2656,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2582,7 +2665,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2591,7 +2674,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2616,7 +2699,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2627,7 +2710,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2636,7 +2719,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2645,7 +2728,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2670,7 +2753,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -2681,7 +2764,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2690,7 +2773,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2699,7 +2782,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2724,12 +2807,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -2740,23 +2823,18 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -2764,6 +2842,11 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Terminé">
@@ -2826,19 +2909,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2849,11 +2932,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2862,7 +2945,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2873,7 +2956,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2882,7 +2965,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2891,7 +2974,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2900,7 +2983,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2909,7 +2992,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2934,7 +3017,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2945,7 +3028,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2954,7 +3037,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2963,7 +3046,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2988,7 +3071,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2999,7 +3082,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3008,7 +3091,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3017,7 +3100,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3042,7 +3125,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3053,7 +3136,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3062,7 +3145,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3071,7 +3154,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3096,7 +3179,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3107,7 +3190,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3116,7 +3199,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3125,7 +3208,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3150,12 +3233,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3166,23 +3249,18 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -3190,6 +3268,11 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Terminé">
@@ -3252,19 +3335,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3275,11 +3358,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3288,7 +3371,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3299,7 +3382,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3308,7 +3391,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3317,7 +3400,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3326,7 +3409,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3335,7 +3418,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3360,7 +3443,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3371,7 +3454,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3380,7 +3463,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3389,7 +3472,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3414,7 +3497,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3425,7 +3508,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3434,7 +3517,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3443,7 +3526,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3468,7 +3551,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3479,7 +3562,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3488,7 +3571,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3497,7 +3580,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3522,7 +3605,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3533,7 +3616,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3542,7 +3625,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3551,7 +3634,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3576,12 +3659,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3592,15 +3675,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3680,19 +3763,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3703,11 +3786,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3716,7 +3799,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3727,7 +3810,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3736,7 +3819,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3745,7 +3828,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3754,7 +3837,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3763,7 +3846,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3788,7 +3871,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3799,7 +3882,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3808,7 +3891,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3817,7 +3900,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3842,7 +3925,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3853,7 +3936,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3862,7 +3945,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3871,7 +3954,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3896,7 +3979,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3907,7 +3990,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3916,7 +3999,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3925,7 +4008,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3950,7 +4033,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3961,7 +4044,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3970,7 +4053,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3979,7 +4062,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4004,12 +4087,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4020,15 +4103,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4106,19 +4189,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -4129,11 +4212,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -4142,7 +4225,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -4153,7 +4236,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4162,7 +4245,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4171,7 +4254,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -4180,7 +4263,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4189,7 +4272,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4214,7 +4297,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="44" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -4225,7 +4308,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -4234,7 +4317,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -4243,7 +4326,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -4268,7 +4351,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -4279,7 +4362,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -4288,7 +4371,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -4297,7 +4380,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -4322,7 +4405,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -4333,7 +4416,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -4342,7 +4425,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4351,7 +4434,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4376,7 +4459,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -4387,7 +4470,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4396,7 +4479,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4405,7 +4488,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4430,12 +4513,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4446,15 +4529,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Modifications Altium et sur la doc
J'ai ajouté toutes les empreintes nécessaires et fait les changement dans la documentation par rapport au dimensionnement
</commit_message>
<xml_diff>
--- a/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
+++ b/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/alexandre_bourquenoud_studentfr_ch/Documents/PHIE/jeu_du_moulin_alexandre_bourquenoud/jeu_du_moulin_2025_boura/jeu_du_moulin_boura/rpt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="13_ncr:1_{C89F1C62-A35A-4363-963D-04F3CDCC9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84A218C9-2E24-4A84-924B-E0D295C4F96D}"/>
+  <xr:revisionPtr revIDLastSave="533" documentId="13_ncr:1_{C89F1C62-A35A-4363-963D-04F3CDCC9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5BA126-42C9-440E-9150-E0D7AEDC4031}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -134,9 +134,6 @@
     <t>quelques problème avec l'implémentation de l'utilisation de Github à cause d'une erreur de setup que j'ai fait avec les repositories -&gt; j'ai résolue le problème en créant correctement les repositories</t>
   </si>
   <si>
-    <t>Documentation</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Rédaction du journal de travail</t>
   </si>
   <si>
-    <t>J'ai pris un bon moment pour faire le symbole de l'uC</t>
-  </si>
-  <si>
     <t>Avancement du schéma -&gt; changement d'IC, ajout  des LEDs manquantes, création des symboles manquants, schématisation des condensateurs de découplage et des matrices de LEDs et de touches capacitives</t>
   </si>
   <si>
@@ -177,6 +171,27 @@
   </si>
   <si>
     <t>création de certaines empreintes manquantes</t>
+  </si>
+  <si>
+    <t>documentation des procédés et actions réalisé au long de la journée</t>
+  </si>
+  <si>
+    <t>J'ai pris un bon moment pour faire le symbole de l'uC car je n'ai pas trouvé celui que j'utilise en ligne</t>
+  </si>
+  <si>
+    <t>Dicsussion avec M. Berset pour l'implementation d'un calcul de la capacité des touches</t>
+  </si>
+  <si>
+    <t>dimensionnement des composants pour le régulateur de tension 3.3V et calcul de consommation du circuit pour choisir le regulateur.</t>
+  </si>
+  <si>
+    <t>documentation avec les nouvelles informations acquéris et documentation des tâches entreprise aujourd'hui -&gt; dimensionnement, changement dans le schéma et BOM</t>
+  </si>
+  <si>
+    <t>Creation et assignement des empreintes au symbols manquant. J'ai aussi fini tous les changement nécessaire au schéma</t>
+  </si>
+  <si>
+    <t>RPT</t>
   </si>
 </sst>
 </file>
@@ -362,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -454,18 +469,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -495,6 +498,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1138,11 +1159,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="4" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1184,19 +1205,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1207,11 +1228,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1241,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1241,15 +1262,15 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="13">
@@ -1258,18 +1279,18 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="13">
         <v>0.9</v>
@@ -1277,15 +1298,15 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="13">
@@ -1294,15 +1315,15 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="6">
@@ -1311,18 +1332,18 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F10" s="6">
         <v>3.5</v>
@@ -1330,7 +1351,7 @@
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1355,34 +1376,34 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="48" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="6">
-        <v>4</v>
+        <v>3.7</v>
       </c>
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6">
@@ -1390,15 +1411,17 @@
       </c>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+    <row r="15" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="47"/>
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="6">
         <v>1.5</v>
@@ -1406,15 +1429,15 @@
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="6">
@@ -1423,15 +1446,15 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4">
@@ -1440,97 +1463,120 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31">
+    <row r="19" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="47"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="31">
         <v>45790</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F20" s="18">
         <f>SUM(F13:F18)</f>
+        <v>6.95</v>
+      </c>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" s="10" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="6"/>
+      <c r="F21" s="6">
+        <v>2</v>
+      </c>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+    <row r="22" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="40"/>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="6">
+        <v>0.2</v>
+      </c>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+    <row r="23" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="40"/>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="6"/>
+      <c r="F23" s="6">
+        <v>1.5</v>
+      </c>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31">
-        <v>45791</v>
-      </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="18">
-        <f>SUM(F20:F23)</f>
-        <v>0</v>
+    <row r="24" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A24" s="40"/>
+      <c r="B24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="6">
+        <v>0.3</v>
       </c>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="4"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1538,7 +1584,7 @@
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1546,17 +1592,26 @@
       <c r="F26" s="6"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="6"/>
+    <row r="27" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="31">
+        <v>45791</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="18">
+        <f>SUM(F21:F26)</f>
+        <v>4</v>
+      </c>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
+      <c r="A28" s="39" t="s">
+        <v>8</v>
+      </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1564,26 +1619,17 @@
       <c r="F28" s="6"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31">
-        <v>45792</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="18">
-        <f>SUM(F25:F28)</f>
-        <v>0</v>
-      </c>
+    <row r="29" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="40"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="6"/>
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="43" t="s">
-        <v>9</v>
-      </c>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1592,7 +1638,7 @@
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1600,17 +1646,26 @@
       <c r="F31" s="6"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="6"/>
+    <row r="32" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="31">
+        <v>45792</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="18">
+        <f>SUM(F28:F31)</f>
+        <v>0</v>
+      </c>
       <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
+      <c r="A33" s="39" t="s">
+        <v>9</v>
+      </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1618,96 +1673,96 @@
       <c r="F33" s="6"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="31">
+    <row r="34" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="40"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="40"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="40"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="31">
         <v>45793</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="20" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="21">
-        <f>SUM(F30:F33)</f>
+      <c r="F37" s="21">
+        <f>SUM(F33:F36)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42" t="s">
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17" t="s">
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="22">
-        <f>F12+F19+F24+F29+F34</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="37" t="s">
+      <c r="G38" s="22">
+        <f>F12+F20+F27+F32+F37</f>
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
       <c r="B39" s="34"/>
-      <c r="C39" s="36"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="34"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="10"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="35"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="10"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="10"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
+      <c r="A44" s="45"/>
       <c r="B44" s="25"/>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
@@ -1716,7 +1771,7 @@
       <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
+      <c r="A45" s="45"/>
       <c r="B45" s="25"/>
       <c r="C45" s="25"/>
       <c r="D45" s="25"/>
@@ -1725,7 +1780,7 @@
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="45"/>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
       <c r="D46" s="25"/>
@@ -1734,16 +1789,16 @@
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="28"/>
+      <c r="A47" s="45"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="26"/>
       <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="45"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
       <c r="D48" s="25"/>
@@ -1752,7 +1807,7 @@
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="45"/>
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
@@ -1761,16 +1816,16 @@
       <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="26"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="28"/>
       <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
+      <c r="A51" s="45"/>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
       <c r="D51" s="25"/>
@@ -1779,16 +1834,16 @@
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="28"/>
+      <c r="A52" s="45"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="26"/>
       <c r="G52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="33"/>
+      <c r="A53" s="45"/>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
       <c r="D53" s="25"/>
@@ -1797,7 +1852,7 @@
       <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+      <c r="A54" s="45"/>
       <c r="B54" s="25"/>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
@@ -1806,16 +1861,16 @@
       <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="26"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="28"/>
       <c r="G55" s="10"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
+      <c r="A56" s="45"/>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
@@ -1824,16 +1879,16 @@
       <c r="G56" s="10"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="24"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="28"/>
+      <c r="A57" s="45"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="26"/>
       <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
+      <c r="A58" s="45"/>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
       <c r="D58" s="25"/>
@@ -1842,7 +1897,7 @@
       <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="33"/>
+      <c r="A59" s="45"/>
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
       <c r="D59" s="25"/>
@@ -1851,16 +1906,16 @@
       <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="26"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="28"/>
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+      <c r="A61" s="45"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
@@ -1869,16 +1924,16 @@
       <c r="G61" s="10"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="28"/>
+      <c r="A62" s="45"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="26"/>
       <c r="G62" s="10"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="45"/>
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
       <c r="D63" s="25"/>
@@ -1887,7 +1942,7 @@
       <c r="G63" s="10"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="33"/>
+      <c r="A64" s="45"/>
       <c r="B64" s="25"/>
       <c r="C64" s="25"/>
       <c r="D64" s="25"/>
@@ -1896,16 +1951,16 @@
       <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="26"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="28"/>
       <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="33"/>
+      <c r="A66" s="45"/>
       <c r="B66" s="25"/>
       <c r="C66" s="25"/>
       <c r="D66" s="25"/>
@@ -1914,60 +1969,87 @@
       <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="24"/>
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="28"/>
+      <c r="A67" s="45"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="26"/>
       <c r="G67" s="10"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="34"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="28"/>
+      <c r="A68" s="45"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="10"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="35"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="35"/>
+      <c r="A69" s="45"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="10"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="24"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="10"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="43"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="28"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="46"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46"/>
+      <c r="D72" s="46"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="A39:G39"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A13:A19"/>
   </mergeCells>
-  <conditionalFormatting sqref="F19:F34 F5:F16">
+  <conditionalFormatting sqref="F5:F16 F20:F37">
     <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F5)))</formula>
     </cfRule>
@@ -1975,28 +2057,28 @@
       <formula>NOT(ISERROR(SEARCH("En cours",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:F67">
+  <conditionalFormatting sqref="F44:F70">
     <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",F41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",F44)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",F41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",F44)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
+  <conditionalFormatting sqref="G38">
     <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G38)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G68">
+  <conditionalFormatting sqref="G71">
     <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G68)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G71)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G68)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2052,19 +2134,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2075,11 +2157,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2088,7 +2170,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2099,7 +2181,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2108,7 +2190,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2117,7 +2199,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2126,7 +2208,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2135,7 +2217,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2160,7 +2242,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2171,7 +2253,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2180,7 +2262,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2189,7 +2271,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2214,7 +2296,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2226,7 +2308,7 @@
       <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2235,7 +2317,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2244,7 +2326,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2269,7 +2351,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2280,7 +2362,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2290,7 +2372,7 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2300,7 +2382,7 @@
       <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2325,7 +2407,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -2336,7 +2418,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2345,7 +2427,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2354,7 +2436,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2379,12 +2461,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:10" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -2395,15 +2477,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2483,19 +2565,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2506,11 +2588,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2519,7 +2601,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2530,7 +2612,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2539,7 +2621,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2548,7 +2630,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2557,7 +2639,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2566,7 +2648,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2591,7 +2673,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2602,7 +2684,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2611,7 +2693,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2620,7 +2702,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2645,7 +2727,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2656,7 +2738,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2665,7 +2747,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2674,7 +2756,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2699,7 +2781,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2710,7 +2792,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2719,7 +2801,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2728,7 +2810,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2753,7 +2835,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -2764,7 +2846,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2773,7 +2855,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2782,7 +2864,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2807,12 +2889,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -2823,18 +2905,23 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -2842,11 +2929,6 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Terminé">
@@ -2909,19 +2991,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2932,11 +3014,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2945,7 +3027,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2956,7 +3038,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2965,7 +3047,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2974,7 +3056,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2983,7 +3065,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2992,7 +3074,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3017,7 +3099,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3028,7 +3110,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3037,7 +3119,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3046,7 +3128,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3071,7 +3153,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3082,7 +3164,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3091,7 +3173,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3100,7 +3182,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3125,7 +3207,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3136,7 +3218,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3145,7 +3227,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3154,7 +3236,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3179,7 +3261,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3190,7 +3272,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3199,7 +3281,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3208,7 +3290,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3233,12 +3315,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3249,18 +3331,23 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -3268,11 +3355,6 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Terminé">
@@ -3335,19 +3417,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3358,11 +3440,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3371,7 +3453,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3382,7 +3464,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3391,7 +3473,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3400,7 +3482,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3409,7 +3491,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3418,7 +3500,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3443,7 +3525,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3454,7 +3536,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3463,7 +3545,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3472,7 +3554,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3497,7 +3579,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3508,7 +3590,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3517,7 +3599,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3526,7 +3608,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3551,7 +3633,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3562,7 +3644,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3571,7 +3653,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3580,7 +3662,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3605,7 +3687,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3616,7 +3698,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3625,7 +3707,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3634,7 +3716,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3659,12 +3741,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3675,15 +3757,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3763,19 +3845,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3786,11 +3868,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3799,7 +3881,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3810,7 +3892,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3819,7 +3901,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3828,7 +3910,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3837,7 +3919,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3846,7 +3928,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3871,7 +3953,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3882,7 +3964,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3891,7 +3973,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3900,7 +3982,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3925,7 +4007,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3936,7 +4018,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3945,7 +4027,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3954,7 +4036,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3979,7 +4061,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3990,7 +4072,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3999,7 +4081,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4008,7 +4090,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4033,7 +4115,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -4044,7 +4126,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4053,7 +4135,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4062,7 +4144,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4087,12 +4169,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4103,15 +4185,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4189,19 +4271,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -4212,11 +4294,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -4225,7 +4307,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -4236,7 +4318,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4245,7 +4327,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4254,7 +4336,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -4263,7 +4345,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4272,7 +4354,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4297,7 +4379,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -4308,7 +4390,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -4317,7 +4399,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -4326,7 +4408,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -4351,7 +4433,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -4362,7 +4444,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -4371,7 +4453,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -4380,7 +4462,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -4405,7 +4487,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -4416,7 +4498,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -4425,7 +4507,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4434,7 +4516,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4459,7 +4541,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -4470,7 +4552,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4479,7 +4561,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4488,7 +4570,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4513,12 +4595,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4529,15 +4611,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Changement principalement sur altium
avancement du routage (les touches sont toutes routées, la majorité des composants sont placées). changement dans la BOM et dans les empreintes pour la MOSFET channel P
</commit_message>
<xml_diff>
--- a/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
+++ b/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/alexandre_bourquenoud_studentfr_ch/Documents/PHIE/jeu_du_moulin_alexandre_bourquenoud/jeu_du_moulin_2025_boura/jeu_du_moulin_boura/rpt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bourquenouda01\OneDrive - EDUETATFR\PHIE\jeu_du_moulin_alexandre_bourquenoud\jeu_du_moulin_2025_boura\jeu_du_moulin_boura\rpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="533" documentId="13_ncr:1_{C89F1C62-A35A-4363-963D-04F3CDCC9C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5BA126-42C9-440E-9150-E0D7AEDC4031}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F77AD1B-655E-40F7-81BC-FD86898DA849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,72 @@
   </si>
   <si>
     <t>RPT</t>
+  </si>
+  <si>
+    <t>corrections final sur le schéma avant l'envoie au superviseur.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">J'ai oublié comment on changais l'énumeration des feuilles du schéma donc j'ai demandé de l'aide à M. Pittet Loïc -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>C'est sous Annotation-Number Schematic Sheet</t>
+    </r>
+  </si>
+  <si>
+    <t>début de la créeation du layout -&gt; importer les changements du schéma</t>
+  </si>
+  <si>
+    <t>Redimensionnement de la matrice de LED</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le calcul utilisé pour la consomation de courant des LED est fausse -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Recalcul</t>
+    </r>
+  </si>
+  <si>
+    <t>changement d'arrangement de la matrice de LED. La première configuration ne laissais pas la possibilité d'allumer les 2 LEDs du même composant a la fois. J'ai pris comme exemple mon ancien projet pour restructurer la matrice.</t>
+  </si>
+  <si>
+    <t>Layout des Touches sur le PCB. j'ai d'abord garder les mêmes dimension que pour le premier prototype de M. Egli mais je changerai la taille comme celle dans le cahier des charges si nécessaire.</t>
+  </si>
+  <si>
+    <t>remplissage du journal du travail</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Après une plus longue réflexion, j'ai remarquer que ce n'était pas nécessaire d'allumer 2 LEDs en même temps -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Perte de temps relativement élevée</t>
+    </r>
+  </si>
+  <si>
+    <t>Je n'ai pas fait de documentation aujourd'hui donc demain je vais essayer de passer plus de temps sur la rédaction du rapport</t>
+  </si>
+  <si>
+    <t>Placement des autres composant sur la plaque et routage de certaines parties. J'ai notamment réussi a router toutes les toouches et toutes la partie alimentation.</t>
   </si>
 </sst>
 </file>
@@ -499,6 +565,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -510,12 +582,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,10 +958,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -1159,11 +1221,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1438,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1395,7 +1457,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1412,7 +1474,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1429,7 +1491,7 @@
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
@@ -1446,7 +1508,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="47"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1463,7 +1525,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -1480,7 +1542,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1519,7 +1581,7 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" s="14"/>
     </row>
@@ -1540,24 +1602,24 @@
       </c>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="40"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="6">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A24" s="40"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
@@ -1566,133 +1628,205 @@
         <v>30</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" s="40"/>
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="6">
         <v>0.3</v>
       </c>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="6"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A26" s="40"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="6"/>
+      <c r="B26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="6">
+        <v>1.5</v>
+      </c>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31">
+    <row r="27" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="40"/>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="31">
         <v>45791</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="18">
-        <f>SUM(F21:F26)</f>
-        <v>4</v>
-      </c>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="39" t="s">
+      <c r="F28" s="18">
+        <f>SUM(F21:F27)</f>
+        <v>6.95</v>
+      </c>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="B29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="6"/>
+      <c r="F29" s="6">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A30" s="40"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="6"/>
+      <c r="B30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.3</v>
+      </c>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="10" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A31" s="40"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="6"/>
+      <c r="B31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1</v>
+      </c>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31">
-        <v>45792</v>
-      </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="18">
-        <f>SUM(F28:F31)</f>
-        <v>0</v>
+    <row r="32" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="40"/>
+      <c r="B32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="6">
+        <v>2.1</v>
       </c>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+    <row r="33" spans="1:7" s="10" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="40"/>
+      <c r="B33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="6"/>
+      <c r="F33" s="6">
+        <v>3.3</v>
+      </c>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="40"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="F34" s="6"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="6"/>
+    <row r="35" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="31">
+        <v>45792</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="18">
+        <f>SUM(F29:F34)</f>
+        <v>7.0333333333333332</v>
+      </c>
       <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="40"/>
+      <c r="A36" s="39" t="s">
+        <v>9</v>
+      </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1700,96 +1834,96 @@
       <c r="F36" s="6"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="31">
+    <row r="37" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="40"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="40"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="40"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="31">
         <v>45793</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="20" t="s">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="21">
-        <f>SUM(F33:F36)</f>
+      <c r="F40" s="21">
+        <f>SUM(F36:F39)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="38" t="s">
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17" t="s">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="22">
-        <f>F12+F20+F27+F32+F37</f>
-        <v>17.95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="33" t="s">
+      <c r="G41" s="22">
+        <f>F12+F20+F28+F35+F40</f>
+        <v>27.93333333333333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="35"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="10"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="35"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="45"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="10"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="45"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="10"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="45"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="25"/>
       <c r="C47" s="25"/>
       <c r="D47" s="25"/>
@@ -1798,7 +1932,7 @@
       <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="45"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
       <c r="D48" s="25"/>
@@ -1807,7 +1941,7 @@
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="45"/>
+      <c r="A49" s="47"/>
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
@@ -1816,16 +1950,16 @@
       <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="28"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="26"/>
       <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="45"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
       <c r="D51" s="25"/>
@@ -1834,7 +1968,7 @@
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
       <c r="D52" s="25"/>
@@ -1843,16 +1977,16 @@
       <c r="G52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="26"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="28"/>
       <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="25"/>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
@@ -1861,16 +1995,16 @@
       <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="28"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="26"/>
       <c r="G55" s="10"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
@@ -1879,7 +2013,7 @@
       <c r="G56" s="10"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
       <c r="D57" s="25"/>
@@ -1888,16 +2022,16 @@
       <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="45"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="26"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="28"/>
       <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="45"/>
+      <c r="A59" s="47"/>
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
       <c r="D59" s="25"/>
@@ -1906,16 +2040,16 @@
       <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="28"/>
+      <c r="A60" s="47"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="26"/>
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="45"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
@@ -1924,7 +2058,7 @@
       <c r="G61" s="10"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="45"/>
+      <c r="A62" s="47"/>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
       <c r="D62" s="25"/>
@@ -1933,16 +2067,16 @@
       <c r="G62" s="10"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="45"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="26"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="28"/>
       <c r="G63" s="10"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="45"/>
+      <c r="A64" s="47"/>
       <c r="B64" s="25"/>
       <c r="C64" s="25"/>
       <c r="D64" s="25"/>
@@ -1951,16 +2085,16 @@
       <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="24"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="28"/>
+      <c r="A65" s="47"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="26"/>
       <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="45"/>
+      <c r="A66" s="47"/>
       <c r="B66" s="25"/>
       <c r="C66" s="25"/>
       <c r="D66" s="25"/>
@@ -1969,7 +2103,7 @@
       <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="45"/>
+      <c r="A67" s="47"/>
       <c r="B67" s="25"/>
       <c r="C67" s="25"/>
       <c r="D67" s="25"/>
@@ -1978,16 +2112,16 @@
       <c r="G67" s="10"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="45"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="26"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="28"/>
       <c r="G68" s="10"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="45"/>
+      <c r="A69" s="47"/>
       <c r="B69" s="25"/>
       <c r="C69" s="25"/>
       <c r="D69" s="25"/>
@@ -1996,60 +2130,87 @@
       <c r="G69" s="10"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
-      <c r="B70" s="29"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="28"/>
+      <c r="A70" s="47"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="26"/>
       <c r="G70" s="10"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="43"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="43"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="28"/>
+      <c r="A71" s="47"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="10"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="46"/>
-      <c r="B72" s="46"/>
-      <c r="C72" s="46"/>
-      <c r="D72" s="46"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="46"/>
+      <c r="A72" s="47"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="10"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="24"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="10"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="45"/>
+      <c r="B74" s="45"/>
+      <c r="C74" s="45"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="28"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="48"/>
+      <c r="B75" s="48"/>
+      <c r="C75" s="48"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="A42:G42"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A41:D41"/>
     <mergeCell ref="A13:A19"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F16 F20:F37">
+  <conditionalFormatting sqref="F5:F16 F20:F40">
     <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F5)))</formula>
     </cfRule>
@@ -2057,28 +2218,28 @@
       <formula>NOT(ISERROR(SEARCH("En cours",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F44:F70">
+  <conditionalFormatting sqref="F47:F73">
     <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",F44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",F47)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",F44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",F47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
+  <conditionalFormatting sqref="G41">
     <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G41)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G71">
+  <conditionalFormatting sqref="G74">
     <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G74)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G71)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changement BOM et journal de travail
complétion de la semaine 1 de travail et modification de la BOM pour inclure le changement de uC
</commit_message>
<xml_diff>
--- a/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
+++ b/jeu_du_moulin_boura/rpt/jeu-du-moulin-bourquenouda-rpt-journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/alexandre_bourquenoud_studentfr_ch/Documents/PHIE/jeu_du_moulin_alexandre_bourquenoud/jeu_du_moulin_2025_boura/jeu_du_moulin_boura/rpt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{5F77AD1B-655E-40F7-81BC-FD86898DA849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09F3A2E-6F56-4F07-95A2-54B8A77A7A4F}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{5F77AD1B-655E-40F7-81BC-FD86898DA849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85A58703-8C08-45C7-A6BE-FC048B19116A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,26 @@
   </si>
   <si>
     <t>J'ai réalisé relativement tard qu'il y avait 2 plans de masse et non 1 plan de masse et 1 plan de VCC qui est la configuration que j'ai utilisé</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">model de uC choisi non disponible à cause d'un manque de stocks -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>check de compatibilité avec les modèles disponibles cherche chez d'autres fournisseurs</t>
+    </r>
+  </si>
+  <si>
+    <t>remplissage de la BOM et control des composants manquants. Un composant n'était pas disponible alors j'ai du changer de model. À la place du STM32L072</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pour cette première semaine, je pense avoir bien travailler avec  un nombre minime de problèmes rencontré même si je devrais prendre plus de temps a rédiger la documentation mais je peux quand même dire que j'ai un peu d'avance dans le routage malgré une petite confusion qui n'est pas encore résolue. Les changements engendré par cette confusion ne seront pas trop élevé je pense donc même si le routage doit être changé, ça ne prendra pas trop de temps.</t>
   </si>
 </sst>
 </file>
@@ -544,18 +564,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -591,6 +599,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,6 +987,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -1230,18 +1254,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="35" style="1" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
@@ -1276,19 +1300,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1299,11 +1323,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1336,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1333,7 +1357,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1350,7 +1374,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
@@ -1369,7 +1393,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1386,7 +1410,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1403,7 +1427,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1422,7 +1446,7 @@
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1447,7 +1471,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1466,7 +1490,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="48"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1483,7 +1507,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="48"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1500,7 +1524,7 @@
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
@@ -1517,7 +1541,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="48"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1534,7 +1558,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="48"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -1551,7 +1575,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="48"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1576,7 +1600,7 @@
       <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" s="10" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1595,7 +1619,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1612,7 +1636,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1629,7 +1653,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1646,7 +1670,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
@@ -1663,7 +1687,7 @@
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
@@ -1682,7 +1706,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="5" t="s">
         <v>22</v>
       </c>
@@ -1715,7 +1739,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1734,7 +1758,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="5" t="s">
         <v>22</v>
       </c>
@@ -1753,7 +1777,7 @@
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" s="10" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1796,7 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
@@ -1789,7 +1813,7 @@
       <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:7" s="10" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="5" t="s">
         <v>22</v>
       </c>
@@ -1806,7 +1830,7 @@
       <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1833,7 +1857,7 @@
       <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1852,22 +1876,22 @@
       <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="6"/>
+      <c r="F37" s="6">
+        <v>1.5</v>
+      </c>
       <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="44"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="5" t="s">
         <v>22</v>
       </c>
@@ -1885,87 +1909,97 @@
       </c>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="44"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="6"/>
+    <row r="39" spans="1:7" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="40"/>
+      <c r="B39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="6">
+        <v>2</v>
+      </c>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="31">
+    <row r="40" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="40"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="31">
         <v>45793</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="20" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="21">
-        <f>SUM(F36:F39)</f>
-        <v>3.5333333333333337</v>
-      </c>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="42" t="s">
+      <c r="F41" s="21">
+        <f>SUM(F36:F40)</f>
+        <v>7.0333333333333332</v>
+      </c>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17" t="s">
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="22">
-        <f>F12+F20+F28+F35+F40</f>
-        <v>31.466666666666665</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="39"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
+      <c r="G42" s="22">
+        <f>F12+F20+F28+F35+F41</f>
+        <v>34.966666666666661</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="35"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
+      <c r="A46" s="45"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
       <c r="F46" s="23"/>
       <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="10"/>
+      <c r="A47" s="45"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
       <c r="D48" s="25"/>
@@ -1974,7 +2008,7 @@
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="47"/>
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
@@ -1983,7 +2017,7 @@
       <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="25"/>
       <c r="C50" s="25"/>
       <c r="D50" s="25"/>
@@ -1992,7 +2026,7 @@
       <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
       <c r="D51" s="25"/>
@@ -2001,7 +2035,7 @@
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="33"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
       <c r="D52" s="25"/>
@@ -2010,25 +2044,25 @@
       <c r="G52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="24"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="28"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="26"/>
       <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="26"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="28"/>
       <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="25"/>
       <c r="C55" s="25"/>
       <c r="D55" s="25"/>
@@ -2037,7 +2071,7 @@
       <c r="G55" s="10"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
@@ -2046,7 +2080,7 @@
       <c r="G56" s="10"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
+      <c r="A57" s="47"/>
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
       <c r="D57" s="25"/>
@@ -2055,25 +2089,25 @@
       <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="24"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="28"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="26"/>
       <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="33"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="26"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="28"/>
       <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="47"/>
       <c r="B60" s="25"/>
       <c r="C60" s="25"/>
       <c r="D60" s="25"/>
@@ -2082,7 +2116,7 @@
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
@@ -2091,7 +2125,7 @@
       <c r="G61" s="10"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
+      <c r="A62" s="47"/>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
       <c r="D62" s="25"/>
@@ -2100,25 +2134,25 @@
       <c r="G62" s="10"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="24"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="28"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="26"/>
       <c r="G63" s="10"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="33"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="26"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="28"/>
       <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
+      <c r="A65" s="47"/>
       <c r="B65" s="25"/>
       <c r="C65" s="25"/>
       <c r="D65" s="25"/>
@@ -2127,7 +2161,7 @@
       <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="33"/>
+      <c r="A66" s="47"/>
       <c r="B66" s="25"/>
       <c r="C66" s="25"/>
       <c r="D66" s="25"/>
@@ -2136,7 +2170,7 @@
       <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
+      <c r="A67" s="47"/>
       <c r="B67" s="25"/>
       <c r="C67" s="25"/>
       <c r="D67" s="25"/>
@@ -2145,25 +2179,25 @@
       <c r="G67" s="10"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="28"/>
+      <c r="A68" s="47"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="26"/>
       <c r="G68" s="10"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="33"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="26"/>
+      <c r="A69" s="24"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="28"/>
       <c r="G69" s="10"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="33"/>
+      <c r="A70" s="47"/>
       <c r="B70" s="25"/>
       <c r="C70" s="25"/>
       <c r="D70" s="25"/>
@@ -2172,7 +2206,7 @@
       <c r="G70" s="10"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="33"/>
+      <c r="A71" s="47"/>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
       <c r="D71" s="25"/>
@@ -2181,7 +2215,7 @@
       <c r="G71" s="10"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="33"/>
+      <c r="A72" s="47"/>
       <c r="B72" s="25"/>
       <c r="C72" s="25"/>
       <c r="D72" s="25"/>
@@ -2190,35 +2224,56 @@
       <c r="G72" s="10"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="24"/>
-      <c r="B73" s="29"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="28"/>
+      <c r="A73" s="47"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="25"/>
+      <c r="F73" s="26"/>
       <c r="G73" s="10"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="28"/>
+      <c r="A74" s="24"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="10"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="35"/>
+      <c r="A75" s="45"/>
+      <c r="B75" s="45"/>
+      <c r="C75" s="45"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="28"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="48"/>
+      <c r="B76" s="48"/>
+      <c r="C76" s="48"/>
+      <c r="D76" s="48"/>
+      <c r="E76" s="48"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="A43:G43"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -2227,23 +2282,11 @@
     <mergeCell ref="A5:A11"/>
     <mergeCell ref="A21:A27"/>
     <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A42:D42"/>
     <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A75:G75"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A69:A72"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F16 F20:F40">
+  <conditionalFormatting sqref="F5:F16 F20:F41">
     <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F5)))</formula>
     </cfRule>
@@ -2251,32 +2294,32 @@
       <formula>NOT(ISERROR(SEARCH("En cours",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47:F73">
+  <conditionalFormatting sqref="F48:F74">
     <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",F47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",F48)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",F47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",F48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
+  <conditionalFormatting sqref="G42">
     <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G42)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G74">
+  <conditionalFormatting sqref="G75">
     <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G74)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G75)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G74)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2328,19 +2371,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2351,11 +2394,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2364,7 +2407,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2375,7 +2418,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2384,7 +2427,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2393,7 +2436,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2402,7 +2445,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2411,7 +2454,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2436,7 +2479,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2447,7 +2490,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2456,7 +2499,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2465,7 +2508,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2490,7 +2533,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2502,7 +2545,7 @@
       <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2511,7 +2554,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2520,7 +2563,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2545,7 +2588,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2556,7 +2599,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2566,7 +2609,7 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2576,7 +2619,7 @@
       <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -2601,7 +2644,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -2612,7 +2655,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2621,7 +2664,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:10" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2630,7 +2673,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:10" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2655,12 +2698,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:10" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -2671,15 +2714,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2759,19 +2802,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2782,11 +2825,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2795,7 +2838,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -2806,7 +2849,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2815,7 +2858,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2824,7 +2867,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2833,7 +2876,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2842,7 +2885,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2867,7 +2910,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -2878,7 +2921,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2887,7 +2930,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2896,7 +2939,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2921,7 +2964,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -2932,7 +2975,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2941,7 +2984,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2950,7 +2993,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2975,7 +3018,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -2986,7 +3029,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -2995,7 +3038,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3004,7 +3047,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3029,7 +3072,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3040,7 +3083,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3049,7 +3092,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3058,7 +3101,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3083,12 +3126,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3099,18 +3142,23 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -3118,11 +3166,6 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Terminé">
@@ -3185,19 +3228,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3208,11 +3251,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3221,7 +3264,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3232,7 +3275,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3241,7 +3284,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3250,7 +3293,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3259,7 +3302,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3268,7 +3311,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3293,7 +3336,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3304,7 +3347,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3313,7 +3356,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3322,7 +3365,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3347,7 +3390,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3358,7 +3401,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3367,7 +3410,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3376,7 +3419,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3401,7 +3444,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3412,7 +3455,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3421,7 +3464,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3430,7 +3473,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3455,7 +3498,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3466,7 +3509,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3475,7 +3518,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3484,7 +3527,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3509,12 +3552,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3525,18 +3568,23 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A5:A10"/>
@@ -3544,11 +3592,6 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F31">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Terminé">
@@ -3611,19 +3654,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3634,11 +3677,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -3647,7 +3690,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -3658,7 +3701,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3667,7 +3710,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3676,7 +3719,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -3685,7 +3728,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -3694,7 +3737,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3719,7 +3762,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -3730,7 +3773,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -3739,7 +3782,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3748,7 +3791,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3773,7 +3816,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -3784,7 +3827,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -3793,7 +3836,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -3802,7 +3845,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3827,7 +3870,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -3838,7 +3881,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3847,7 +3890,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3856,7 +3899,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -3881,7 +3924,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -3892,7 +3935,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3901,7 +3944,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3910,7 +3953,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -3935,12 +3978,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -3951,15 +3994,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4039,19 +4082,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -4062,11 +4105,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -4075,7 +4118,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -4086,7 +4129,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4095,7 +4138,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4104,7 +4147,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -4113,7 +4156,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4122,7 +4165,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4147,7 +4190,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -4158,7 +4201,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -4167,7 +4210,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -4176,7 +4219,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -4201,7 +4244,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -4212,7 +4255,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -4221,7 +4264,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -4230,7 +4273,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -4255,7 +4298,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -4266,7 +4309,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -4275,7 +4318,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4284,7 +4327,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4309,7 +4352,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -4320,7 +4363,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4329,7 +4372,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4338,7 +4381,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4363,12 +4406,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4379,15 +4422,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4465,19 +4508,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -4488,11 +4531,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
@@ -4501,7 +4544,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -4512,7 +4555,7 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4521,7 +4564,7 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4530,7 +4573,7 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -4539,7 +4582,7 @@
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -4548,7 +4591,7 @@
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4573,7 +4616,7 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
@@ -4584,7 +4627,7 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -4593,7 +4636,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -4602,7 +4645,7 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -4627,7 +4670,7 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4"/>
@@ -4638,7 +4681,7 @@
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -4647,7 +4690,7 @@
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -4656,7 +4699,7 @@
       <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -4681,7 +4724,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="4"/>
@@ -4692,7 +4735,7 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -4701,7 +4744,7 @@
       <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -4710,7 +4753,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4735,7 +4778,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="4"/>
@@ -4746,7 +4789,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4755,7 +4798,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4764,7 +4807,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4789,12 +4832,12 @@
       <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
         <v>12</v>
@@ -4805,15 +4848,15 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>